<commit_message>
Common: Connected mods, cells, cells with cell types and so on
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/cells.xlsx
+++ b/upgrade/fixtures/cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F6F97-4B0D-2D46-8FA3-4DD8D40C3538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEBEBB1-50B4-4F8F-BC83-6231207629DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1540" windowWidth="23960" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="2625" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <t>40T</t>
   </si>
   <si>
-    <t>size</t>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -424,13 +424,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -456,19 +456,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -485,7 +485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -502,7 +502,7 @@
         <v>18650</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -519,7 +519,7 @@
         <v>18650</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -536,7 +536,7 @@
         <v>18650</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>